<commit_message>
Completed the xls xlsx and csv functionality
</commit_message>
<xml_diff>
--- a/testBookLibrary.xlsx
+++ b/testBookLibrary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\programming\softwareEng\bulky-book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F277B8C-0075-4C57-B50D-B1858847B6E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E618211-AD2C-4997-89FC-1B135CEF4B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8385" yWindow="1920" windowWidth="15375" windowHeight="7875" xr2:uid="{A2B74C87-EE24-4496-AB2C-99CCF2945409}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" xr2:uid="{A2B74C87-EE24-4496-AB2C-99CCF2945409}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>UserId</t>
   </si>
@@ -123,6 +123,21 @@
   </si>
   <si>
     <t>Tolu Republica</t>
+  </si>
+  <si>
+    <t>New Book Chapter</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>353-890-545-131</t>
+  </si>
+  <si>
+    <t>Emmanuel</t>
+  </si>
+  <si>
+    <t>Emma Circle</t>
   </si>
 </sst>
 </file>
@@ -475,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB509AF2-91B0-4F88-99EF-E23419E2D2DD}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,6 +640,29 @@
         <v>29</v>
       </c>
     </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>107</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>